<commit_message>
export dữ liệu cho report store unchecked
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Store_Unchecked.xlsx
+++ b/DMS/Templates/Report_Store_Unchecked.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B23730-D609-4AF0-96EF-80690275808D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>STT</t>
   </si>
@@ -42,9 +41,6 @@
     <t>Địa chỉ</t>
   </si>
   <si>
-    <t>Tuyến</t>
-  </si>
-  <si>
     <t>Số điện thoại</t>
   </si>
   <si>
@@ -73,9 +69,6 @@
   </si>
   <si>
     <t>{{ReportStoreUncheckeds.SaleEmployees.Stores.Date}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreUncheckeds.SaleEmployees.Stores.ERouteCode}}</t>
   </si>
   <si>
     <t>{{ReportStoreUncheckeds.SaleEmployees.Stores.StoreCode}}</t>
@@ -111,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,31 +554,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:L4"/>
+      <selection activeCell="A8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="34.6640625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -593,9 +585,8 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -603,11 +594,10 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
     </row>
-    <row r="4" spans="1:18" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -619,30 +609,27 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -658,27 +645,24 @@
         <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -689,59 +673,55 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="7"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>